<commit_message>
Update Math 300 Proposed Syllabus.xlsx
</commit_message>
<xml_diff>
--- a/Admin/Math 300 Proposed Syllabus.xlsx
+++ b/Admin/Math 300 Proposed Syllabus.xlsx
@@ -826,8 +826,8 @@
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1524,11 +1524,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Binding xmlns="72c6b8df-9cc8-43e4-bbbd-f4c12caad843">true</Binding>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1592,7 +1588,11 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Binding xmlns="72c6b8df-9cc8-43e4-bbbd-f4c12caad843">true</Binding>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1605,16 +1605,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24140494-20CC-41C6-B8AE-61FD12F99C6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC62554B-1B75-408E-916B-6415182A4C31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="72c6b8df-9cc8-43e4-bbbd-f4c12caad843"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1637,9 +1630,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC62554B-1B75-408E-916B-6415182A4C31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24140494-20CC-41C6-B8AE-61FD12F99C6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="72c6b8df-9cc8-43e4-bbbd-f4c12caad843"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>